<commit_message>
add event action - make a copy of existing event config instead of using latest event template
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/minister_designation/001-Minister_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/minister_designation/001-Minister_Designation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\minister_designation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\epictrack-api\src\api\templates\event_templates\minister_designation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2137BD0A-780E-414E-98C6-1D929FC7A0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE6D333-7FA1-4545-AEA2-61C44D5DB2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -32,8 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -516,9 +514,6 @@
     <t>Event Position</t>
   </si>
   <si>
-    <t>MutipleDays</t>
-  </si>
-  <si>
     <t>EventPosition</t>
   </si>
   <si>
@@ -796,6 +791,9 @@
   </si>
   <si>
     <t>{"work_state": "COMPLETED"}</t>
+  </si>
+  <si>
+    <t>MultipleDays</t>
   </si>
 </sst>
 </file>
@@ -1350,55 +1348,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
       <c r="C3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>64</v>
       </c>
@@ -1419,18 +1417,18 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="14.77734375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1456,12 +1454,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -1482,12 +1480,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>9</v>
@@ -1508,12 +1506,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
@@ -1567,29 +1565,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E014DF34-0612-424C-AA89-DB5D1D4ABE25}">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="10.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.77734375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.77734375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1612,10 +1610,10 @@
         <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>30</v>
@@ -1630,7 +1628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1638,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" s="6" t="str">
         <f>IF((C2=""),"",VLOOKUP(C2,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1669,7 +1667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1677,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="6" t="str">
         <f>IF((C3=""),"",VLOOKUP(C3,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1708,7 +1706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1716,7 +1714,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="6" t="str">
         <f>IF((C4=""),"",VLOOKUP(C4,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1747,7 +1745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1755,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="6" t="str">
         <f>IF((C5=""),"",VLOOKUP(C5,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1786,7 +1784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1794,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E6" s="6" t="str">
         <f>IF((C6=""),"",VLOOKUP(C6,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1825,7 +1823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1864,7 +1862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1872,14 +1870,14 @@
         <v>1</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" s="6" t="str">
         <f>IF((C8=""),"",VLOOKUP(C8,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Intake</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>34</v>
@@ -1903,7 +1901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1911,7 +1909,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="6" t="str">
         <f>IF((C9=""),"",VLOOKUP(C9,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1942,7 +1940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1950,7 +1948,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="6" t="str">
         <f>IF((C10=""),"",VLOOKUP(C10,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1981,7 +1979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1989,7 +1987,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E11" s="6" t="str">
         <f>IF((C11=""),"",VLOOKUP(C11,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2020,7 +2018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2028,7 +2026,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E12" s="6" t="str">
         <f>IF((C12=""),"",VLOOKUP(C12,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2059,7 +2057,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2067,7 +2065,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E13" s="6" t="str">
         <f>IF((C13=""),"",VLOOKUP(C13,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2098,7 +2096,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2109,7 +2107,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E14" s="6" t="str">
         <f>IF((C14=""),"",VLOOKUP(C14,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2140,7 +2138,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2151,7 +2149,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E15" s="6" t="str">
         <f>IF((C15=""),"",VLOOKUP(C15,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2182,7 +2180,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2193,7 +2191,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E16" s="6" t="str">
         <f>IF((C16=""),"",VLOOKUP(C16,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2224,7 +2222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2235,7 +2233,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E17" s="6" t="str">
         <f>IF((C17=""),"",VLOOKUP(C17,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2266,7 +2264,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2305,7 +2303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2344,7 +2342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2352,7 +2350,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E20" s="6" t="str">
         <f>IF((C20=""),"",VLOOKUP(C20,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2383,7 +2381,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2394,7 +2392,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E21" s="6" t="str">
         <f>IF((C21=""),"",VLOOKUP(C21,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2425,7 +2423,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2436,7 +2434,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E22" s="6" t="str">
         <f>IF((C22=""),"",VLOOKUP(C22,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2467,7 +2465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2475,7 +2473,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E23" s="6" t="str">
         <f>IF((C23=""),"",VLOOKUP(C23,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2506,7 +2504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2517,7 +2515,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E24" s="6" t="str">
         <f>IF((C24=""),"",VLOOKUP(C24,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2548,7 +2546,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2559,7 +2557,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E25" s="6" t="str">
         <f>IF((C25=""),"",VLOOKUP(C25,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2590,7 +2588,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2598,7 +2596,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E26" s="6" t="str">
         <f>IF((C26=""),"",VLOOKUP(C26,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2629,7 +2627,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2640,7 +2638,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E27" s="6" t="str">
         <f>IF((C27=""),"",VLOOKUP(C27,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2671,7 +2669,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2682,7 +2680,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E28" s="6" t="str">
         <f>IF((C28=""),"",VLOOKUP(C28,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2713,7 +2711,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2721,14 +2719,14 @@
         <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E29" s="6" t="str">
         <f>IF((C29=""),"",VLOOKUP(C29,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>40</v>
@@ -2752,7 +2750,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2763,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E30" s="6" t="str">
         <f>IF((C30=""),"",VLOOKUP(C30,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2794,7 +2792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2805,7 +2803,7 @@
         <v>2</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E31" s="6" t="str">
         <f>IF((C31=""),"",VLOOKUP(C31,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2836,7 +2834,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2844,7 +2842,7 @@
         <v>2</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E32" s="6" t="str">
         <f>IF((C32=""),"",VLOOKUP(C32,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2875,7 +2873,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2886,7 +2884,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E33" s="6" t="str">
         <f>IF((C33=""),"",VLOOKUP(C33,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2917,7 +2915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2928,7 +2926,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E34" s="6" t="str">
         <f>IF((C34=""),"",VLOOKUP(C34,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2959,7 +2957,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2967,7 +2965,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E35" s="6" t="str">
         <f>IF((C35=""),"",VLOOKUP(C35,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2998,7 +2996,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3009,7 +3007,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E36" s="6" t="str">
         <f>IF((C36=""),"",VLOOKUP(C36,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3040,7 +3038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3051,7 +3049,7 @@
         <v>2</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E37" s="6" t="str">
         <f>IF((C37=""),"",VLOOKUP(C37,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3082,7 +3080,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3121,7 +3119,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3129,7 +3127,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E39" s="6" t="str">
         <f>IF((C39=""),"",VLOOKUP(C39,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3160,7 +3158,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3168,7 +3166,7 @@
         <v>3</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E40" s="6" t="str">
         <f>IF((C40=""),"",VLOOKUP(C40,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3199,7 +3197,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3207,7 +3205,7 @@
         <v>3</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E41" s="6" t="str">
         <f>IF((C41=""),"",VLOOKUP(C41,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3238,7 +3236,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3249,7 +3247,7 @@
         <v>3</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E42" s="6" t="str">
         <f>IF((C42=""),"",VLOOKUP(C42,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3280,7 +3278,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3288,7 +3286,7 @@
         <v>3</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E43" s="6" t="str">
         <f>IF((C43=""),"",VLOOKUP(C43,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3319,7 +3317,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3327,7 +3325,7 @@
         <v>3</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E44" s="6" t="str">
         <f>IF((C44=""),"",VLOOKUP(C44,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3358,7 +3356,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3369,7 +3367,7 @@
         <v>3</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E45" s="6" t="str">
         <f>IF((C45=""),"",VLOOKUP(C45,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3400,7 +3398,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3411,7 +3409,7 @@
         <v>3</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E46" s="6" t="str">
         <f>IF((C46=""),"",VLOOKUP(C46,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3442,7 +3440,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3450,7 +3448,7 @@
         <v>3</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E47" s="6" t="str">
         <f>IF((C47=""),"",VLOOKUP(C47,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3481,7 +3479,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3492,7 +3490,7 @@
         <v>3</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E48" s="6" t="str">
         <f>IF((C48=""),"",VLOOKUP(C48,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3523,7 +3521,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3534,7 +3532,7 @@
         <v>3</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E49" s="6" t="str">
         <f>IF((C49=""),"",VLOOKUP(C49,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3565,7 +3563,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3573,7 +3571,7 @@
         <v>3</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E50" s="6" t="str">
         <f>IF((C50=""),"",VLOOKUP(C50,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3604,7 +3602,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3615,7 +3613,7 @@
         <v>3</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E51" s="6" t="str">
         <f>IF((C51=""),"",VLOOKUP(C51,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3646,7 +3644,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3657,7 +3655,7 @@
         <v>3</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E52" s="6" t="str">
         <f>IF((C52=""),"",VLOOKUP(C52,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3688,7 +3686,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3727,7 +3725,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -3735,7 +3733,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E54" s="6" t="str">
         <f>IF((C54=""),"",VLOOKUP(C54,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3766,7 +3764,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -3777,7 +3775,7 @@
         <v>3</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E55" s="6" t="str">
         <f>IF((C55=""),"",VLOOKUP(C55,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3808,7 +3806,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -3819,7 +3817,7 @@
         <v>3</v>
       </c>
       <c r="D56" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E56" s="6" t="str">
         <f>IF((C56=""),"",VLOOKUP(C56,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3916,16 +3914,16 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="70.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="70.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3942,7 +3940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3954,13 +3952,13 @@
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3972,13 +3970,13 @@
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3990,13 +3988,13 @@
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4008,13 +4006,13 @@
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4026,13 +4024,13 @@
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4044,13 +4042,13 @@
         <v>Minister's Designation Application Received</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4062,13 +4060,13 @@
         <v>Delegation of Decision</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4080,13 +4078,13 @@
         <v>Delegation of Decision</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4098,13 +4096,13 @@
         <v>Minister's Designation Process Terminated s.39(d)</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4116,13 +4114,13 @@
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4134,13 +4132,13 @@
         <v>Minister's Designation Process Terminated s.39(d)</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E12" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4152,13 +4150,13 @@
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E13" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4170,13 +4168,13 @@
         <v>Minister's Designation Decision</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E14" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4188,7 +4186,7 @@
         <v>Minister's Designation Decision</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E15" s="3">
         <v>14</v>
@@ -4215,26 +4213,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="12.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="70.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="107.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="107.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4257,7 +4255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4269,19 +4267,19 @@
         <v>Draft Minister's Designation Application is "incomplete"</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>161</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -4293,19 +4291,19 @@
         <v>Draft Minister's Designation Application is "incomplete"</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4317,19 +4315,19 @@
         <v>Draft Minister's Designation Application is for an "eligible" project</v>
       </c>
       <c r="D4" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>164</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4341,19 +4339,19 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D5" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4365,19 +4363,19 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4389,19 +4387,19 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4413,10 +4411,10 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D8" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>173</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>174</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>66</v>
@@ -4425,7 +4423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4437,19 +4435,19 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D9" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4461,19 +4459,19 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4485,19 +4483,19 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4509,19 +4507,19 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D12" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4533,19 +4531,19 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4557,10 +4555,10 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D14" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>168</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>169</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>66</v>
@@ -4569,7 +4567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4581,19 +4579,19 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D15" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G15" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -4605,19 +4603,19 @@
         <v>Starts the "clock" for Minister's Designation</v>
       </c>
       <c r="D16" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>176</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G16" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -4629,19 +4627,19 @@
         <v>Minister is delegated to make the final Minister's Designation Decision</v>
       </c>
       <c r="D17" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="E17" s="22" t="s">
-        <v>178</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G17" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -4653,19 +4651,19 @@
         <v>CEAO is delegated to make the final Minister's Designation Decision</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G18" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4677,19 +4675,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D19" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E19" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G19" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -4701,19 +4699,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G20" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4725,19 +4723,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G21" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -4749,19 +4747,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D22" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E22" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G22" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -4773,19 +4771,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D23" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E23" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E23" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G23" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -4797,19 +4795,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G24" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -4821,19 +4819,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D25" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E25" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="E25" s="22" t="s">
-        <v>169</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G25" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -4845,19 +4843,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D26" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E26" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E26" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G26" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -4869,19 +4867,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D27" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E27" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E27" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G27" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -4893,19 +4891,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G28" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -4917,19 +4915,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G29" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -4941,19 +4939,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D30" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E30" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E30" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G30" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -4965,19 +4963,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D31" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E31" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F31" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G31" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -4989,19 +4987,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G32" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -5013,19 +5011,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D33" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E33" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="E33" s="22" t="s">
-        <v>169</v>
-      </c>
       <c r="F33" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G33" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -5037,19 +5035,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D34" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E34" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G34" s="3">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -5061,19 +5059,19 @@
         <v>Decision Maker Designates Project as Reviewable</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G35" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -5085,10 +5083,10 @@
         <v>Decision Maker Designates Project as Reviewable</v>
       </c>
       <c r="D36" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" s="22" t="s">
         <v>173</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>174</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>66</v>
@@ -5097,7 +5095,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -5109,19 +5107,19 @@
         <v>Decision Maker Declines to Designate Project as Reviewable</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G37" s="3">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -5133,13 +5131,13 @@
         <v>Decision Maker Declines to Designate Project as Reviewable</v>
       </c>
       <c r="D38" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E38" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E38" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G38" s="3">
         <v>37</v>
@@ -5173,34 +5171,34 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.77734375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="3.77734375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.77734375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.77734375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.77734375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.77734375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.77734375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.77734375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="30.77734375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="3.77734375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.77734375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.77734375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.77734375" style="4" customWidth="1"/>
-    <col min="20" max="58" width="3.77734375" style="4" customWidth="1"/>
-    <col min="59" max="59" width="8.88671875" style="4"/>
-    <col min="60" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="3.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.7109375" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="4" customWidth="1"/>
+    <col min="20" max="58" width="3.7109375" style="4" customWidth="1"/>
+    <col min="59" max="59" width="8.85546875" style="4"/>
+    <col min="60" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -5236,7 +5234,7 @@
       </c>
       <c r="R2" s="5"/>
       <c r="S2" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -5279,7 +5277,7 @@
       <c r="BF2" s="5"/>
       <c r="BG2" s="5"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
@@ -5305,13 +5303,13 @@
         <v>52</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S3" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -5343,7 +5341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
@@ -5366,7 +5364,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
@@ -5383,9 +5381,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>34</v>
@@ -5400,7 +5398,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -5417,9 +5415,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>34</v>
@@ -5434,7 +5432,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
@@ -5448,7 +5446,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
@@ -5460,7 +5458,7 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
@@ -5468,11 +5466,11 @@
         <v>34</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
@@ -5484,7 +5482,7 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
@@ -5496,7 +5494,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
@@ -5508,7 +5506,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
@@ -5516,10 +5514,10 @@
         <v>40</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H17" s="4" t="s">
         <v>36</v>
       </c>
@@ -5527,7 +5525,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="4" t="s">
         <v>36</v>
       </c>
@@ -5535,7 +5533,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H19" s="4" t="s">
         <v>36</v>
       </c>
@@ -5543,7 +5541,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H20" s="4" t="s">
         <v>36</v>
       </c>
@@ -5551,7 +5549,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H21" s="4" t="s">
         <v>36</v>
       </c>
@@ -5559,7 +5557,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H22" s="4" t="s">
         <v>36</v>
       </c>
@@ -5567,7 +5565,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H23" s="4" t="s">
         <v>36</v>
       </c>
@@ -5575,7 +5573,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H24" s="4" t="s">
         <v>36</v>
       </c>
@@ -5583,7 +5581,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H25" s="4" t="s">
         <v>36</v>
       </c>
@@ -5591,7 +5589,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H26" s="4" t="s">
         <v>38</v>
       </c>
@@ -5599,7 +5597,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H27" s="4" t="s">
         <v>38</v>
       </c>
@@ -5607,7 +5605,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H28" s="4" t="s">
         <v>38</v>
       </c>
@@ -5615,7 +5613,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H29" s="4" t="s">
         <v>38</v>
       </c>
@@ -5623,7 +5621,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H30" s="4" t="s">
         <v>35</v>
       </c>
@@ -5631,7 +5629,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H31" s="4" t="s">
         <v>35</v>
       </c>
@@ -5639,7 +5637,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H32" s="4" t="s">
         <v>35</v>
       </c>
@@ -5647,7 +5645,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33" s="4" t="s">
         <v>35</v>
       </c>
@@ -5655,7 +5653,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34" s="4" t="s">
         <v>35</v>
       </c>
@@ -5663,7 +5661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35" s="4" t="s">
         <v>37</v>
       </c>
@@ -5671,7 +5669,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H36" s="4" t="s">
         <v>37</v>
       </c>
@@ -5679,7 +5677,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H37" s="4" t="s">
         <v>37</v>
       </c>
@@ -5687,7 +5685,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H38" s="4" t="s">
         <v>37</v>
       </c>
@@ -5695,7 +5693,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H39" s="4" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
#1134 - Complex Actions (#1166)
* #1134 - Complex Actions

added action handlers for following:
  - AddEvent
  - AddPhase
  - CreateWork
  - SetEventDate

* linting fixes

* work plan - sort phases based on ID instead of sort order

* amend last commit

* add event action - make a copy of existing event config instead of using latest event template
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/minister_designation/001-Minister_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/minister_designation/001-Minister_Designation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\minister_designation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\aot\EPIC-FLOW\epictrack-api\src\api\templates\event_templates\minister_designation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2137BD0A-780E-414E-98C6-1D929FC7A0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE6D333-7FA1-4545-AEA2-61C44D5DB2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -32,8 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -516,9 +514,6 @@
     <t>Event Position</t>
   </si>
   <si>
-    <t>MutipleDays</t>
-  </si>
-  <si>
     <t>EventPosition</t>
   </si>
   <si>
@@ -796,6 +791,9 @@
   </si>
   <si>
     <t>{"work_state": "COMPLETED"}</t>
+  </si>
+  <si>
+    <t>MultipleDays</t>
   </si>
 </sst>
 </file>
@@ -1350,55 +1348,55 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
       <c r="C3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>64</v>
       </c>
@@ -1419,18 +1417,18 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="14.77734375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1456,12 +1454,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -1482,12 +1480,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>9</v>
@@ -1508,12 +1506,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
@@ -1567,29 +1565,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E014DF34-0612-424C-AA89-DB5D1D4ABE25}">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="3" customWidth="1"/>
-    <col min="2" max="3" width="10.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.77734375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="14.77734375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="14.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1612,10 +1610,10 @@
         <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>30</v>
@@ -1630,7 +1628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1638,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" s="6" t="str">
         <f>IF((C2=""),"",VLOOKUP(C2,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1669,7 +1667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1677,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="6" t="str">
         <f>IF((C3=""),"",VLOOKUP(C3,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1708,7 +1706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1716,7 +1714,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="6" t="str">
         <f>IF((C4=""),"",VLOOKUP(C4,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1747,7 +1745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1755,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="6" t="str">
         <f>IF((C5=""),"",VLOOKUP(C5,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1786,7 +1784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1794,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E6" s="6" t="str">
         <f>IF((C6=""),"",VLOOKUP(C6,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1825,7 +1823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1864,7 +1862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1872,14 +1870,14 @@
         <v>1</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" s="6" t="str">
         <f>IF((C8=""),"",VLOOKUP(C8,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Intake</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>34</v>
@@ -1903,7 +1901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1911,7 +1909,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="6" t="str">
         <f>IF((C9=""),"",VLOOKUP(C9,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1942,7 +1940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1950,7 +1948,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="6" t="str">
         <f>IF((C10=""),"",VLOOKUP(C10,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -1981,7 +1979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1989,7 +1987,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E11" s="6" t="str">
         <f>IF((C11=""),"",VLOOKUP(C11,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2020,7 +2018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2028,7 +2026,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E12" s="6" t="str">
         <f>IF((C12=""),"",VLOOKUP(C12,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2059,7 +2057,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2067,7 +2065,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E13" s="6" t="str">
         <f>IF((C13=""),"",VLOOKUP(C13,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2098,7 +2096,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2109,7 +2107,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E14" s="6" t="str">
         <f>IF((C14=""),"",VLOOKUP(C14,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2140,7 +2138,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2151,7 +2149,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E15" s="6" t="str">
         <f>IF((C15=""),"",VLOOKUP(C15,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2182,7 +2180,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2193,7 +2191,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E16" s="6" t="str">
         <f>IF((C16=""),"",VLOOKUP(C16,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2224,7 +2222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2235,7 +2233,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E17" s="6" t="str">
         <f>IF((C17=""),"",VLOOKUP(C17,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2266,7 +2264,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2305,7 +2303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2344,7 +2342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2352,7 +2350,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E20" s="6" t="str">
         <f>IF((C20=""),"",VLOOKUP(C20,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2383,7 +2381,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2394,7 +2392,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E21" s="6" t="str">
         <f>IF((C21=""),"",VLOOKUP(C21,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2425,7 +2423,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2436,7 +2434,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E22" s="6" t="str">
         <f>IF((C22=""),"",VLOOKUP(C22,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2467,7 +2465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2475,7 +2473,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E23" s="6" t="str">
         <f>IF((C23=""),"",VLOOKUP(C23,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2506,7 +2504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2517,7 +2515,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E24" s="6" t="str">
         <f>IF((C24=""),"",VLOOKUP(C24,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2548,7 +2546,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2559,7 +2557,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E25" s="6" t="str">
         <f>IF((C25=""),"",VLOOKUP(C25,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2590,7 +2588,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2598,7 +2596,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E26" s="6" t="str">
         <f>IF((C26=""),"",VLOOKUP(C26,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2629,7 +2627,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2640,7 +2638,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E27" s="6" t="str">
         <f>IF((C27=""),"",VLOOKUP(C27,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2671,7 +2669,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2682,7 +2680,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E28" s="6" t="str">
         <f>IF((C28=""),"",VLOOKUP(C28,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2713,7 +2711,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2721,14 +2719,14 @@
         <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E29" s="6" t="str">
         <f>IF((C29=""),"",VLOOKUP(C29,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>40</v>
@@ -2752,7 +2750,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2763,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E30" s="6" t="str">
         <f>IF((C30=""),"",VLOOKUP(C30,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2794,7 +2792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2805,7 +2803,7 @@
         <v>2</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E31" s="6" t="str">
         <f>IF((C31=""),"",VLOOKUP(C31,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2836,7 +2834,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2844,7 +2842,7 @@
         <v>2</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E32" s="6" t="str">
         <f>IF((C32=""),"",VLOOKUP(C32,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2875,7 +2873,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2886,7 +2884,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E33" s="6" t="str">
         <f>IF((C33=""),"",VLOOKUP(C33,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2917,7 +2915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2928,7 +2926,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E34" s="6" t="str">
         <f>IF((C34=""),"",VLOOKUP(C34,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2959,7 +2957,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2967,7 +2965,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E35" s="6" t="str">
         <f>IF((C35=""),"",VLOOKUP(C35,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2998,7 +2996,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3009,7 +3007,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E36" s="6" t="str">
         <f>IF((C36=""),"",VLOOKUP(C36,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3040,7 +3038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3051,7 +3049,7 @@
         <v>2</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E37" s="6" t="str">
         <f>IF((C37=""),"",VLOOKUP(C37,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3082,7 +3080,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3121,7 +3119,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3129,7 +3127,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E39" s="6" t="str">
         <f>IF((C39=""),"",VLOOKUP(C39,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3160,7 +3158,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3168,7 +3166,7 @@
         <v>3</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E40" s="6" t="str">
         <f>IF((C40=""),"",VLOOKUP(C40,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3199,7 +3197,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3207,7 +3205,7 @@
         <v>3</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E41" s="6" t="str">
         <f>IF((C41=""),"",VLOOKUP(C41,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3238,7 +3236,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3249,7 +3247,7 @@
         <v>3</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E42" s="6" t="str">
         <f>IF((C42=""),"",VLOOKUP(C42,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3280,7 +3278,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3288,7 +3286,7 @@
         <v>3</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E43" s="6" t="str">
         <f>IF((C43=""),"",VLOOKUP(C43,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3319,7 +3317,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3327,7 +3325,7 @@
         <v>3</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E44" s="6" t="str">
         <f>IF((C44=""),"",VLOOKUP(C44,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3358,7 +3356,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3369,7 +3367,7 @@
         <v>3</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E45" s="6" t="str">
         <f>IF((C45=""),"",VLOOKUP(C45,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3400,7 +3398,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3411,7 +3409,7 @@
         <v>3</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E46" s="6" t="str">
         <f>IF((C46=""),"",VLOOKUP(C46,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3442,7 +3440,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3450,7 +3448,7 @@
         <v>3</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E47" s="6" t="str">
         <f>IF((C47=""),"",VLOOKUP(C47,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3481,7 +3479,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3492,7 +3490,7 @@
         <v>3</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E48" s="6" t="str">
         <f>IF((C48=""),"",VLOOKUP(C48,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3523,7 +3521,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3534,7 +3532,7 @@
         <v>3</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E49" s="6" t="str">
         <f>IF((C49=""),"",VLOOKUP(C49,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3565,7 +3563,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3573,7 +3571,7 @@
         <v>3</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E50" s="6" t="str">
         <f>IF((C50=""),"",VLOOKUP(C50,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3604,7 +3602,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3615,7 +3613,7 @@
         <v>3</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E51" s="6" t="str">
         <f>IF((C51=""),"",VLOOKUP(C51,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3646,7 +3644,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3657,7 +3655,7 @@
         <v>3</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E52" s="6" t="str">
         <f>IF((C52=""),"",VLOOKUP(C52,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3688,7 +3686,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3727,7 +3725,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -3735,7 +3733,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E54" s="6" t="str">
         <f>IF((C54=""),"",VLOOKUP(C54,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3766,7 +3764,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -3777,7 +3775,7 @@
         <v>3</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E55" s="6" t="str">
         <f>IF((C55=""),"",VLOOKUP(C55,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3808,7 +3806,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -3819,7 +3817,7 @@
         <v>3</v>
       </c>
       <c r="D56" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E56" s="6" t="str">
         <f>IF((C56=""),"",VLOOKUP(C56,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -3916,16 +3914,16 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="70.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="6.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="70.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3942,7 +3940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3954,13 +3952,13 @@
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3972,13 +3970,13 @@
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3990,13 +3988,13 @@
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4008,13 +4006,13 @@
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4026,13 +4024,13 @@
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4044,13 +4042,13 @@
         <v>Minister's Designation Application Received</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4062,13 +4060,13 @@
         <v>Delegation of Decision</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4080,13 +4078,13 @@
         <v>Delegation of Decision</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4098,13 +4096,13 @@
         <v>Minister's Designation Process Terminated s.39(d)</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4116,13 +4114,13 @@
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4134,13 +4132,13 @@
         <v>Minister's Designation Process Terminated s.39(d)</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E12" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4152,13 +4150,13 @@
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E13" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4170,13 +4168,13 @@
         <v>Minister's Designation Decision</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E14" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4188,7 +4186,7 @@
         <v>Minister's Designation Decision</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E15" s="3">
         <v>14</v>
@@ -4215,26 +4213,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="12.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="70.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="107.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="107.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4257,7 +4255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4269,19 +4267,19 @@
         <v>Draft Minister's Designation Application is "incomplete"</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>161</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -4293,19 +4291,19 @@
         <v>Draft Minister's Designation Application is "incomplete"</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4317,19 +4315,19 @@
         <v>Draft Minister's Designation Application is for an "eligible" project</v>
       </c>
       <c r="D4" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>164</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4341,19 +4339,19 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D5" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4365,19 +4363,19 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4389,19 +4387,19 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4413,10 +4411,10 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D8" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>173</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>174</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>66</v>
@@ -4425,7 +4423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4437,19 +4435,19 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D9" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4461,19 +4459,19 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4485,19 +4483,19 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4509,19 +4507,19 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D12" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4533,19 +4531,19 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4557,10 +4555,10 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D14" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>168</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>169</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>66</v>
@@ -4569,7 +4567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4581,19 +4579,19 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D15" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G15" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -4605,19 +4603,19 @@
         <v>Starts the "clock" for Minister's Designation</v>
       </c>
       <c r="D16" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>176</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G16" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -4629,19 +4627,19 @@
         <v>Minister is delegated to make the final Minister's Designation Decision</v>
       </c>
       <c r="D17" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="E17" s="22" t="s">
-        <v>178</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G17" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -4653,19 +4651,19 @@
         <v>CEAO is delegated to make the final Minister's Designation Decision</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G18" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4677,19 +4675,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D19" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E19" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G19" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -4701,19 +4699,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G20" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4725,19 +4723,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G21" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -4749,19 +4747,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D22" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E22" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G22" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -4773,19 +4771,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D23" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E23" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E23" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G23" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -4797,19 +4795,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G24" s="3">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -4821,19 +4819,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D25" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E25" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="E25" s="22" t="s">
-        <v>169</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G25" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -4845,19 +4843,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D26" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E26" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E26" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G26" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -4869,19 +4867,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D27" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E27" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E27" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G27" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -4893,19 +4891,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G28" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -4917,19 +4915,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G29" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -4941,19 +4939,19 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D30" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E30" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E30" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G30" s="3">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -4965,19 +4963,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D31" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E31" s="22" t="s">
-        <v>166</v>
-      </c>
       <c r="F31" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G31" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -4989,19 +4987,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G32" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -5013,19 +5011,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D33" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E33" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="E33" s="22" t="s">
-        <v>169</v>
-      </c>
       <c r="F33" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G33" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -5037,19 +5035,19 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D34" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E34" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G34" s="3">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -5061,19 +5059,19 @@
         <v>Decision Maker Designates Project as Reviewable</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G35" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -5085,10 +5083,10 @@
         <v>Decision Maker Designates Project as Reviewable</v>
       </c>
       <c r="D36" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" s="22" t="s">
         <v>173</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>174</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>66</v>
@@ -5097,7 +5095,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -5109,19 +5107,19 @@
         <v>Decision Maker Declines to Designate Project as Reviewable</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G37" s="3">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -5133,13 +5131,13 @@
         <v>Decision Maker Declines to Designate Project as Reviewable</v>
       </c>
       <c r="D38" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E38" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E38" s="22" t="s">
-        <v>171</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G38" s="3">
         <v>37</v>
@@ -5173,34 +5171,34 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="3.77734375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="3.77734375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="3.77734375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.77734375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="3.77734375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.77734375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3.77734375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3.77734375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="30.77734375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="3.77734375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="14.77734375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="3.77734375" style="4" customWidth="1"/>
-    <col min="19" max="19" width="14.77734375" style="4" customWidth="1"/>
-    <col min="20" max="58" width="3.77734375" style="4" customWidth="1"/>
-    <col min="59" max="59" width="8.88671875" style="4"/>
-    <col min="60" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="3.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" style="4" customWidth="1"/>
+    <col min="18" max="18" width="3.7109375" style="4" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="4" customWidth="1"/>
+    <col min="20" max="58" width="3.7109375" style="4" customWidth="1"/>
+    <col min="59" max="59" width="8.85546875" style="4"/>
+    <col min="60" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -5236,7 +5234,7 @@
       </c>
       <c r="R2" s="5"/>
       <c r="S2" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -5279,7 +5277,7 @@
       <c r="BF2" s="5"/>
       <c r="BG2" s="5"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
@@ -5305,13 +5303,13 @@
         <v>52</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S3" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -5343,7 +5341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
@@ -5366,7 +5364,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
@@ -5383,9 +5381,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>34</v>
@@ -5400,7 +5398,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -5417,9 +5415,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>34</v>
@@ -5434,7 +5432,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
@@ -5448,7 +5446,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
@@ -5460,7 +5458,7 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
@@ -5468,11 +5466,11 @@
         <v>34</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
@@ -5484,7 +5482,7 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
@@ -5496,7 +5494,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
@@ -5508,7 +5506,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
@@ -5516,10 +5514,10 @@
         <v>40</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H17" s="4" t="s">
         <v>36</v>
       </c>
@@ -5527,7 +5525,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="4" t="s">
         <v>36</v>
       </c>
@@ -5535,7 +5533,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H19" s="4" t="s">
         <v>36</v>
       </c>
@@ -5543,7 +5541,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H20" s="4" t="s">
         <v>36</v>
       </c>
@@ -5551,7 +5549,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H21" s="4" t="s">
         <v>36</v>
       </c>
@@ -5559,7 +5557,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H22" s="4" t="s">
         <v>36</v>
       </c>
@@ -5567,7 +5565,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H23" s="4" t="s">
         <v>36</v>
       </c>
@@ -5575,7 +5573,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H24" s="4" t="s">
         <v>36</v>
       </c>
@@ -5583,7 +5581,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H25" s="4" t="s">
         <v>36</v>
       </c>
@@ -5591,7 +5589,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H26" s="4" t="s">
         <v>38</v>
       </c>
@@ -5599,7 +5597,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H27" s="4" t="s">
         <v>38</v>
       </c>
@@ -5607,7 +5605,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H28" s="4" t="s">
         <v>38</v>
       </c>
@@ -5615,7 +5613,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H29" s="4" t="s">
         <v>38</v>
       </c>
@@ -5623,7 +5621,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H30" s="4" t="s">
         <v>35</v>
       </c>
@@ -5631,7 +5629,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H31" s="4" t="s">
         <v>35</v>
       </c>
@@ -5639,7 +5637,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H32" s="4" t="s">
         <v>35</v>
       </c>
@@ -5647,7 +5645,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33" s="4" t="s">
         <v>35</v>
       </c>
@@ -5655,7 +5653,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34" s="4" t="s">
         <v>35</v>
       </c>
@@ -5663,7 +5661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35" s="4" t="s">
         <v>37</v>
       </c>
@@ -5671,7 +5669,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H36" s="4" t="s">
         <v>37</v>
       </c>
@@ -5679,7 +5677,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H37" s="4" t="s">
         <v>37</v>
       </c>
@@ -5687,7 +5685,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H38" s="4" t="s">
         <v>37</v>
       </c>
@@ -5695,7 +5693,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H39" s="4" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
removing suspension and resumption
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/minister_designation/001-Minister_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/minister_designation/001-Minister_Designation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\minister_designation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5834CDDA-0EB8-4F37-B682-6DBB151AEF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5790C5-4F76-4CB1-97D8-DDEF6B65A977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="192">
   <si>
     <t>No</t>
   </si>
@@ -607,16 +607,10 @@
     <t>Time Limit Extended Milestone Bullet</t>
   </si>
   <si>
-    <t>s.45 Suspension of the Minister's Designation Process</t>
-  </si>
-  <si>
     <t>Minister's Designation Process Suspension Announcement &amp; Tweet</t>
   </si>
   <si>
     <t>Minister's Designation Process Suspended Milestone Bullet</t>
-  </si>
-  <si>
-    <t>s.45 Resumption of the Minister's Designation Process</t>
   </si>
   <si>
     <t>Minister's Designation Process Resumption Announcement &amp; Tweet</t>
@@ -1563,13 +1557,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E014DF34-0612-424C-AA89-DB5D1D4ABE25}">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1613,7 +1607,7 @@
         <v>100</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>30</v>
@@ -2590,12 +2584,15 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
+        <v>26</v>
+      </c>
+      <c r="B26" s="3">
         <v>25</v>
       </c>
       <c r="C26" s="8">
         <v>2</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="18" t="s">
         <v>131</v>
       </c>
       <c r="E26" s="6" t="str">
@@ -2603,10 +2600,10 @@
         <v>Minister's Designation Review</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>98</v>
@@ -2624,12 +2621,12 @@
         <v>0</v>
       </c>
       <c r="M26" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3">
         <v>25</v>
@@ -2637,7 +2634,7 @@
       <c r="C27" s="8">
         <v>2</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="19" t="s">
         <v>132</v>
       </c>
       <c r="E27" s="6" t="str">
@@ -2645,7 +2642,7 @@
         <v>Minister's Designation Review</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>35</v>
@@ -2666,20 +2663,20 @@
         <v>0</v>
       </c>
       <c r="M27" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" s="3">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C28" s="8">
         <v>2</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="18" t="s">
         <v>133</v>
       </c>
       <c r="E28" s="6" t="str">
@@ -2687,7 +2684,7 @@
         <v>Minister's Designation Review</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>35</v>
@@ -2708,17 +2705,20 @@
         <v>0</v>
       </c>
       <c r="M28" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
+        <v>30</v>
+      </c>
+      <c r="B29" s="3">
         <v>28</v>
       </c>
       <c r="C29" s="8">
         <v>2</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="19" t="s">
         <v>134</v>
       </c>
       <c r="E29" s="6" t="str">
@@ -2726,10 +2726,10 @@
         <v>Minister's Designation Review</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>98</v>
@@ -2747,20 +2747,17 @@
         <v>0</v>
       </c>
       <c r="M29" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>29</v>
-      </c>
-      <c r="B30" s="3">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C30" s="8">
         <v>2</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="17" t="s">
         <v>135</v>
       </c>
       <c r="E30" s="6" t="str">
@@ -2768,10 +2765,10 @@
         <v>Minister's Designation Review</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>98</v>
@@ -2789,20 +2786,20 @@
         <v>0</v>
       </c>
       <c r="M30" s="3">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31" s="3">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C31" s="8">
         <v>2</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="18" t="s">
         <v>136</v>
       </c>
       <c r="E31" s="6" t="str">
@@ -2810,7 +2807,7 @@
         <v>Minister's Designation Review</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>35</v>
@@ -2831,17 +2828,20 @@
         <v>0</v>
       </c>
       <c r="M31" s="3">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
+        <v>33</v>
+      </c>
+      <c r="B32" s="3">
         <v>31</v>
       </c>
       <c r="C32" s="8">
         <v>2</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="19" t="s">
         <v>137</v>
       </c>
       <c r="E32" s="6" t="str">
@@ -2849,10 +2849,10 @@
         <v>Minister's Designation Review</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>98</v>
@@ -2870,31 +2870,28 @@
         <v>0</v>
       </c>
       <c r="M32" s="3">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>32</v>
-      </c>
-      <c r="B33" s="3">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C33" s="8">
         <v>2</v>
       </c>
-      <c r="D33" s="18" t="s">
-        <v>138</v>
+      <c r="D33" s="17" t="s">
+        <v>115</v>
       </c>
       <c r="E33" s="6" t="str">
         <f>IF((C33=""),"",VLOOKUP(C33,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>98</v>
@@ -2912,28 +2909,28 @@
         <v>0</v>
       </c>
       <c r="M33" s="3">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" s="3">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C34" s="8">
         <v>2</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>139</v>
+      <c r="D34" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="E34" s="6" t="str">
         <f>IF((C34=""),"",VLOOKUP(C34,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>35</v>
@@ -2954,28 +2951,31 @@
         <v>0</v>
       </c>
       <c r="M34" s="3">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
+        <v>36</v>
+      </c>
+      <c r="B35" s="3">
         <v>34</v>
       </c>
       <c r="C35" s="8">
         <v>2</v>
       </c>
-      <c r="D35" s="17" t="s">
-        <v>115</v>
+      <c r="D35" s="19" t="s">
+        <v>139</v>
       </c>
       <c r="E35" s="6" t="str">
         <f>IF((C35=""),"",VLOOKUP(C35,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>98</v>
@@ -2993,31 +2993,28 @@
         <v>0</v>
       </c>
       <c r="M35" s="3">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>35</v>
-      </c>
-      <c r="B36" s="3">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C36" s="8">
         <v>2</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>140</v>
+      <c r="D36" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E36" s="6" t="str">
         <f>IF((C36=""),"",VLOOKUP(C36,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>98</v>
@@ -3035,31 +3032,28 @@
         <v>0</v>
       </c>
       <c r="M36" s="3">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C37" s="8">
         <v>2</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>141</v>
+      <c r="D37" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="E37" s="6" t="str">
         <f>IF((C37=""),"",VLOOKUP(C37,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>98</v>
@@ -3068,34 +3062,34 @@
         <v>0</v>
       </c>
       <c r="J37" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K37" s="3">
         <v>0</v>
       </c>
       <c r="L37" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" s="3">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C38" s="8">
-        <v>2</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>140</v>
       </c>
       <c r="E38" s="6" t="str">
         <f>IF((C38=""),"",VLOOKUP(C38,Phases!$A$2:$B$4,2,FALSE))</f>
-        <v>Minister's Designation Review</v>
+        <v>Minister's Designation Decision</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>34</v>
@@ -3113,28 +3107,28 @@
         <v>0</v>
       </c>
       <c r="L38" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" s="3">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C39" s="8">
-        <v>2</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>118</v>
+        <v>3</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="E39" s="6" t="str">
         <f>IF((C39=""),"",VLOOKUP(C39,Phases!$A$2:$B$4,2,FALSE))</f>
-        <v>Minister's Designation Review</v>
+        <v>Minister's Designation Decision</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>34</v>
@@ -3146,7 +3140,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="2">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="K39" s="3">
         <v>0</v>
@@ -3155,17 +3149,20 @@
         <v>1</v>
       </c>
       <c r="M39" s="3">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="B40" s="3">
+        <v>40</v>
       </c>
       <c r="C40" s="8">
         <v>3</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="19" t="s">
         <v>142</v>
       </c>
       <c r="E40" s="6" t="str">
@@ -3173,10 +3170,10 @@
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>98</v>
@@ -3194,25 +3191,25 @@
         <v>1</v>
       </c>
       <c r="M40" s="3">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C41" s="8">
         <v>3</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="E41" s="6" t="str">
         <f>IF((C41=""),"",VLOOKUP(C41,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>34</v>
@@ -3224,40 +3221,37 @@
         <v>0</v>
       </c>
       <c r="J41" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K41" s="3">
         <v>0</v>
       </c>
       <c r="L41" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41" s="3">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
-        <v>41</v>
-      </c>
-      <c r="B42" s="3">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C42" s="8">
         <v>3</v>
       </c>
-      <c r="D42" s="19" t="s">
-        <v>144</v>
+      <c r="D42" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="E42" s="6" t="str">
         <f>IF((C42=""),"",VLOOKUP(C42,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H42" s="7" t="s">
         <v>98</v>
@@ -3272,31 +3266,34 @@
         <v>0</v>
       </c>
       <c r="L42" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" s="3">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B43" s="3">
+        <v>43</v>
       </c>
       <c r="C43" s="8">
         <v>3</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>114</v>
+      <c r="D43" s="18" t="s">
+        <v>129</v>
       </c>
       <c r="E43" s="6" t="str">
         <f>IF((C43=""),"",VLOOKUP(C43,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>98</v>
@@ -3314,28 +3311,31 @@
         <v>0</v>
       </c>
       <c r="M43" s="3">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
+        <v>45</v>
+      </c>
+      <c r="B44" s="3">
         <v>43</v>
       </c>
       <c r="C44" s="8">
         <v>3</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>128</v>
+      <c r="D44" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="E44" s="6" t="str">
         <f>IF((C44=""),"",VLOOKUP(C44,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>98</v>
@@ -3353,31 +3353,28 @@
         <v>0</v>
       </c>
       <c r="M44" s="3">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
-        <v>44</v>
-      </c>
-      <c r="B45" s="3">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C45" s="8">
         <v>3</v>
       </c>
-      <c r="D45" s="18" t="s">
-        <v>129</v>
+      <c r="D45" s="17" t="s">
+        <v>135</v>
       </c>
       <c r="E45" s="6" t="str">
         <f>IF((C45=""),"",VLOOKUP(C45,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>98</v>
@@ -3395,28 +3392,28 @@
         <v>0</v>
       </c>
       <c r="M45" s="3">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B46" s="3">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C46" s="8">
         <v>3</v>
       </c>
-      <c r="D46" s="19" t="s">
-        <v>130</v>
+      <c r="D46" s="18" t="s">
+        <v>136</v>
       </c>
       <c r="E46" s="6" t="str">
         <f>IF((C46=""),"",VLOOKUP(C46,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>35</v>
@@ -3437,17 +3434,20 @@
         <v>0</v>
       </c>
       <c r="M46" s="3">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
+        <v>48</v>
+      </c>
+      <c r="B47" s="3">
         <v>46</v>
       </c>
       <c r="C47" s="8">
         <v>3</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="19" t="s">
         <v>137</v>
       </c>
       <c r="E47" s="6" t="str">
@@ -3455,10 +3455,10 @@
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>98</v>
@@ -3476,31 +3476,28 @@
         <v>0</v>
       </c>
       <c r="M47" s="3">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
-        <v>47</v>
-      </c>
-      <c r="B48" s="3">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C48" s="8">
         <v>3</v>
       </c>
-      <c r="D48" s="18" t="s">
-        <v>138</v>
+      <c r="D48" s="17" t="s">
+        <v>115</v>
       </c>
       <c r="E48" s="6" t="str">
         <f>IF((C48=""),"",VLOOKUP(C48,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>98</v>
@@ -3518,28 +3515,28 @@
         <v>0</v>
       </c>
       <c r="M48" s="3">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49" s="3">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C49" s="8">
         <v>3</v>
       </c>
-      <c r="D49" s="19" t="s">
-        <v>139</v>
+      <c r="D49" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="E49" s="6" t="str">
         <f>IF((C49=""),"",VLOOKUP(C49,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>35</v>
@@ -3560,28 +3557,31 @@
         <v>0</v>
       </c>
       <c r="M49" s="3">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
+        <v>51</v>
+      </c>
+      <c r="B50" s="3">
         <v>49</v>
       </c>
       <c r="C50" s="8">
         <v>3</v>
       </c>
-      <c r="D50" s="17" t="s">
-        <v>115</v>
+      <c r="D50" s="19" t="s">
+        <v>139</v>
       </c>
       <c r="E50" s="6" t="str">
         <f>IF((C50=""),"",VLOOKUP(C50,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H50" s="7" t="s">
         <v>98</v>
@@ -3599,31 +3599,28 @@
         <v>0</v>
       </c>
       <c r="M50" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>50</v>
-      </c>
-      <c r="B51" s="3">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C51" s="8">
         <v>3</v>
       </c>
-      <c r="D51" s="18" t="s">
-        <v>140</v>
+      <c r="D51" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E51" s="6" t="str">
         <f>IF((C51=""),"",VLOOKUP(C51,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>98</v>
@@ -3641,31 +3638,28 @@
         <v>0</v>
       </c>
       <c r="M51" s="3">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <v>51</v>
-      </c>
-      <c r="B52" s="3">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C52" s="8">
         <v>3</v>
       </c>
-      <c r="D52" s="19" t="s">
-        <v>141</v>
+      <c r="D52" s="21" t="s">
+        <v>109</v>
       </c>
       <c r="E52" s="6" t="str">
         <f>IF((C52=""),"",VLOOKUP(C52,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>98</v>
@@ -3674,37 +3668,40 @@
         <v>0</v>
       </c>
       <c r="J52" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K52" s="3">
         <v>0</v>
       </c>
       <c r="L52" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M52" s="3">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="B53" s="3">
+        <v>53</v>
       </c>
       <c r="C53" s="8">
         <v>3</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>19</v>
+      <c r="D53" s="18" t="s">
+        <v>143</v>
       </c>
       <c r="E53" s="6" t="str">
         <f>IF((C53=""),"",VLOOKUP(C53,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>98</v>
@@ -3719,31 +3716,34 @@
         <v>0</v>
       </c>
       <c r="L53" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M53" s="3">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
+        <v>55</v>
+      </c>
+      <c r="B54" s="3">
         <v>53</v>
       </c>
       <c r="C54" s="8">
         <v>3</v>
       </c>
-      <c r="D54" s="21" t="s">
-        <v>109</v>
+      <c r="D54" s="19" t="s">
+        <v>144</v>
       </c>
       <c r="E54" s="6" t="str">
         <f>IF((C54=""),"",VLOOKUP(C54,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>98</v>
@@ -3752,7 +3752,7 @@
         <v>0</v>
       </c>
       <c r="J54" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K54" s="3">
         <v>0</v>
@@ -3761,95 +3761,11 @@
         <v>1</v>
       </c>
       <c r="M54" s="3">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A55" s="3">
-        <v>54</v>
-      </c>
-      <c r="B55" s="3">
-        <v>53</v>
-      </c>
-      <c r="C55" s="8">
-        <v>3</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="E55" s="6" t="str">
-        <f>IF((C55=""),"",VLOOKUP(C55,Phases!$A$2:$B$4,2,FALSE))</f>
-        <v>Minister's Designation Decision</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="I55" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J55" s="2">
-        <v>0</v>
-      </c>
-      <c r="K55" s="3">
-        <v>0</v>
-      </c>
-      <c r="L55" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M55" s="3">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A56" s="3">
         <v>55</v>
       </c>
-      <c r="B56" s="3">
-        <v>53</v>
-      </c>
-      <c r="C56" s="8">
-        <v>3</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E56" s="6" t="str">
-        <f>IF((C56=""),"",VLOOKUP(C56,Phases!$A$2:$B$4,2,FALSE))</f>
-        <v>Minister's Designation Decision</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H56" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="I56" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J56" s="2">
-        <v>0</v>
-      </c>
-      <c r="K56" s="3">
-        <v>0</v>
-      </c>
-      <c r="L56" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M56" s="3">
-        <v>55</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H56">
+  <conditionalFormatting sqref="H1:H54">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="END">
       <formula>NOT(ISERROR(SEARCH("END",H1)))</formula>
     </cfRule>
@@ -3865,37 +3781,37 @@
           <x14:formula1>
             <xm:f>Lookups!$M$3:$M$4</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L56</xm:sqref>
+          <xm:sqref>L2:L54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{52DB5617-9AC6-42B3-A0A1-82418CF13405}">
           <x14:formula1>
             <xm:f>Lookups!$K$3:$K$9</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G56</xm:sqref>
+          <xm:sqref>G2:G54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{65DF4310-1509-4DE8-8535-DCDB722824BD}">
           <x14:formula1>
             <xm:f>Lookups!$Q$3:$Q$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H56</xm:sqref>
+          <xm:sqref>H2:H54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6E633788-78DC-4B8E-B8EE-32416443C2DA}">
           <x14:formula1>
             <xm:f>Lookups!$S$3:$S$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I56</xm:sqref>
+          <xm:sqref>I2:I54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{486DEDE7-BAAD-4F07-BF86-68CC65BA16B7}">
           <x14:formula1>
             <xm:f>Lookups!$I$3:$I$39</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F56</xm:sqref>
+          <xm:sqref>F2:F54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{22B15D01-845E-49E3-A9EB-3C108A48B871}">
           <x14:formula1>
             <xm:f>Phases!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C56</xm:sqref>
+          <xm:sqref>C2:C54</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3948,11 +3864,11 @@
         <v>3</v>
       </c>
       <c r="C2" s="6" t="str">
-        <f>IF((B2=""),"",VLOOKUP(B2,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B2=""),"",VLOOKUP(B2,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -3966,11 +3882,11 @@
         <v>3</v>
       </c>
       <c r="C3" s="6" t="str">
-        <f>IF((B3=""),"",VLOOKUP(B3,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B3=""),"",VLOOKUP(B3,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -3984,11 +3900,11 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="str">
-        <f>IF((B4=""),"",VLOOKUP(B4,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B4=""),"",VLOOKUP(B4,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E4" s="3">
         <v>3</v>
@@ -4002,11 +3918,11 @@
         <v>3</v>
       </c>
       <c r="C5" s="6" t="str">
-        <f>IF((B5=""),"",VLOOKUP(B5,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B5=""),"",VLOOKUP(B5,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
@@ -4020,11 +3936,11 @@
         <v>5</v>
       </c>
       <c r="C6" s="6" t="str">
-        <f>IF((B6=""),"",VLOOKUP(B6,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B6=""),"",VLOOKUP(B6,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E6" s="3">
         <v>5</v>
@@ -4038,11 +3954,11 @@
         <v>8</v>
       </c>
       <c r="C7" s="6" t="str">
-        <f>IF((B7=""),"",VLOOKUP(B7,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B7=""),"",VLOOKUP(B7,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Received</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E7" s="3">
         <v>6</v>
@@ -4056,11 +3972,11 @@
         <v>9</v>
       </c>
       <c r="C8" s="6" t="str">
-        <f>IF((B8=""),"",VLOOKUP(B8,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B8=""),"",VLOOKUP(B8,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Delegation of Decision</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E8" s="3">
         <v>7</v>
@@ -4074,11 +3990,11 @@
         <v>9</v>
       </c>
       <c r="C9" s="6" t="str">
-        <f>IF((B9=""),"",VLOOKUP(B9,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B9=""),"",VLOOKUP(B9,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Delegation of Decision</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E9" s="3">
         <v>8</v>
@@ -4092,11 +4008,11 @@
         <v>31</v>
       </c>
       <c r="C10" s="6" t="str">
-        <f>IF((B10=""),"",VLOOKUP(B10,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B10=""),"",VLOOKUP(B10,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Process Terminated s.39(d)</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E10" s="3">
         <v>9</v>
@@ -4110,11 +4026,11 @@
         <v>34</v>
       </c>
       <c r="C11" s="6" t="str">
-        <f>IF((B11=""),"",VLOOKUP(B11,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B11=""),"",VLOOKUP(B11,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E11" s="3">
         <v>10</v>
@@ -4128,11 +4044,11 @@
         <v>46</v>
       </c>
       <c r="C12" s="6" t="str">
-        <f>IF((B12=""),"",VLOOKUP(B12,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B12=""),"",VLOOKUP(B12,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Process Terminated s.39(d)</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E12" s="3">
         <v>11</v>
@@ -4146,11 +4062,11 @@
         <v>49</v>
       </c>
       <c r="C13" s="6" t="str">
-        <f>IF((B13=""),"",VLOOKUP(B13,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B13=""),"",VLOOKUP(B13,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E13" s="3">
         <v>12</v>
@@ -4164,11 +4080,11 @@
         <v>53</v>
       </c>
       <c r="C14" s="6" t="str">
-        <f>IF((B14=""),"",VLOOKUP(B14,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B14=""),"",VLOOKUP(B14,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E14" s="3">
         <v>13</v>
@@ -4182,11 +4098,11 @@
         <v>53</v>
       </c>
       <c r="C15" s="6" t="str">
-        <f>IF((B15=""),"",VLOOKUP(B15,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B15=""),"",VLOOKUP(B15,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E15" s="3">
         <v>14</v>
@@ -4199,7 +4115,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{104E34E7-1558-4F0E-B347-AA979B498781}">
           <x14:formula1>
-            <xm:f>Events!$A$2:$A$56</xm:f>
+            <xm:f>Events!$A$2:$A$54</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B15</xm:sqref>
         </x14:dataValidation>
@@ -4213,7 +4129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A29F23-3414-4C7A-B10C-DD605B945639}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -4267,13 +4183,13 @@
         <v>Draft Minister's Designation Application is "incomplete"</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -4291,13 +4207,13 @@
         <v>Draft Minister's Designation Application is "incomplete"</v>
       </c>
       <c r="D3" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>161</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -4315,13 +4231,13 @@
         <v>Draft Minister's Designation Application is for an "eligible" project</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
@@ -4339,13 +4255,13 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -4363,13 +4279,13 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
@@ -4387,13 +4303,13 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
@@ -4411,10 +4327,10 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>66</v>
@@ -4435,13 +4351,13 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
@@ -4459,13 +4375,13 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
@@ -4483,13 +4399,13 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
@@ -4507,13 +4423,13 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
@@ -4531,13 +4447,13 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
@@ -4555,10 +4471,10 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>66</v>
@@ -4579,13 +4495,13 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G15" s="3">
         <v>14</v>
@@ -4603,13 +4519,13 @@
         <v>Starts the "clock" for Minister's Designation</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G16" s="3">
         <v>15</v>
@@ -4627,13 +4543,13 @@
         <v>Minister is delegated to make the final Minister's Designation Decision</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G17" s="3">
         <v>16</v>
@@ -4651,13 +4567,13 @@
         <v>CEAO is delegated to make the final Minister's Designation Decision</v>
       </c>
       <c r="D18" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="E18" s="22" t="s">
-        <v>178</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G18" s="3">
         <v>17</v>
@@ -4675,13 +4591,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G19" s="3">
         <v>18</v>
@@ -4699,13 +4615,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G20" s="3">
         <v>19</v>
@@ -4723,13 +4639,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G21" s="3">
         <v>20</v>
@@ -4747,13 +4663,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G22" s="3">
         <v>21</v>
@@ -4771,13 +4687,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G23" s="3">
         <v>22</v>
@@ -4795,13 +4711,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G24" s="3">
         <v>23</v>
@@ -4819,13 +4735,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G25" s="3">
         <v>24</v>
@@ -4843,13 +4759,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G26" s="3">
         <v>25</v>
@@ -4867,13 +4783,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G27" s="3">
         <v>26</v>
@@ -4891,13 +4807,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G28" s="3">
         <v>27</v>
@@ -4915,13 +4831,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G29" s="3">
         <v>28</v>
@@ -4939,13 +4855,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G30" s="3">
         <v>29</v>
@@ -4963,13 +4879,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G31" s="3">
         <v>30</v>
@@ -4987,13 +4903,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G32" s="3">
         <v>31</v>
@@ -5011,13 +4927,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G33" s="3">
         <v>32</v>
@@ -5035,13 +4951,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G34" s="3">
         <v>33</v>
@@ -5059,13 +4975,13 @@
         <v>Decision Maker Designates Project as Reviewable</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G35" s="3">
         <v>34</v>
@@ -5083,10 +4999,10 @@
         <v>Decision Maker Designates Project as Reviewable</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>66</v>
@@ -5107,13 +5023,13 @@
         <v>Decision Maker Declines to Designate Project as Reviewable</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G37" s="3">
         <v>36</v>
@@ -5131,13 +5047,13 @@
         <v>Decision Maker Declines to Designate Project as Reviewable</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G38" s="3">
         <v>37</v>

</xml_diff>

<commit_message>
change in actions, event templates (#1290)
* project notification template updated + master templates added

* removing suspension and resumption

* template changes/ assessment template

* - Create API to import data from Excels to master tables - #1204
   - Created APIs to import:
     - indigenous nations
     - projects
     - proponents
     - staff
   - Added migration script to load new look up data
 - Added new field bcgid to indigenous nations
 - Actions now send time converted PST to respective service calls
 - Removed redundant session.commit() from actions
 - Added new project state values 'CLOSED', 'UNDER_DESIGNATION'

* actions, change in templates

---------

Co-authored-by: salabh-an <salabh.n@aot-technologies.com>
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/minister_designation/001-Minister_Designation.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/minister_designation/001-Minister_Designation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\minister_designation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5834CDDA-0EB8-4F37-B682-6DBB151AEF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC048CF-A7D8-4FD0-B3DD-0635D08E3C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="197">
   <si>
     <t>No</t>
   </si>
@@ -412,9 +412,6 @@
     <t>#FFFFFF</t>
   </si>
   <si>
-    <t>{}</t>
-  </si>
-  <si>
     <t>Generic</t>
   </si>
   <si>
@@ -607,18 +604,12 @@
     <t>Time Limit Extended Milestone Bullet</t>
   </si>
   <si>
-    <t>s.45 Suspension of the Minister's Designation Process</t>
-  </si>
-  <si>
     <t>Minister's Designation Process Suspension Announcement &amp; Tweet</t>
   </si>
   <si>
     <t>Minister's Designation Process Suspended Milestone Bullet</t>
   </si>
   <si>
-    <t>s.45 Resumption of the Minister's Designation Process</t>
-  </si>
-  <si>
     <t>Minister's Designation Process Resumption Announcement &amp; Tweet</t>
   </si>
   <si>
@@ -794,6 +785,24 @@
   </si>
   <si>
     <t>{"phase_name":"Minister's Designation Review","work_type_id": 2, "ea_act_id": 3, "event_name": "Minister's Designation Application Received", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>Visibility</t>
+  </si>
+  <si>
+    <t>REGULAR</t>
+  </si>
+  <si>
+    <t>MANDATORY</t>
+  </si>
+  <si>
+    <t>OPTIONAL</t>
+  </si>
+  <si>
+    <t>{"all_future_phases":false}</t>
+  </si>
+  <si>
+    <t>{"work_type":6}</t>
   </si>
 </sst>
 </file>
@@ -1408,13 +1417,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8789B1A8-4095-496B-ABDA-23EBF7B52DFC}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1423,12 +1432,12 @@
     <col min="2" max="2" width="50.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" style="2" customWidth="1"/>
     <col min="4" max="5" width="14.6640625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="6" max="8" width="12.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1451,15 +1460,18 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -1476,16 +1488,19 @@
       <c r="G2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>9</v>
@@ -1502,16 +1517,19 @@
       <c r="G3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
@@ -1528,7 +1546,10 @@
       <c r="G4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I4" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1563,13 +1584,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E014DF34-0612-424C-AA89-DB5D1D4ABE25}">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1581,8 +1602,7 @@
     <col min="6" max="6" width="32.6640625" style="2" customWidth="1"/>
     <col min="7" max="9" width="14.6640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" style="2" customWidth="1"/>
+    <col min="11" max="12" width="14.6640625" style="2" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" style="2" customWidth="1"/>
     <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
@@ -1610,10 +1630,10 @@
         <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>30</v>
@@ -1622,7 +1642,7 @@
         <v>4</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>31</v>
+        <v>191</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>7</v>
@@ -1636,20 +1656,20 @@
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" s="6" t="str">
         <f>IF((C2=""),"",VLOOKUP(C2,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Intake</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I2" s="7" t="b">
         <v>0</v>
@@ -1660,8 +1680,8 @@
       <c r="K2" s="3">
         <v>0</v>
       </c>
-      <c r="L2" s="8" t="b">
-        <v>1</v>
+      <c r="L2" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M2" s="3">
         <v>1</v>
@@ -1675,20 +1695,20 @@
         <v>1</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="6" t="str">
         <f>IF((C3=""),"",VLOOKUP(C3,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Intake</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I3" s="7" t="b">
         <v>0</v>
@@ -1699,8 +1719,8 @@
       <c r="K3" s="3">
         <v>0</v>
       </c>
-      <c r="L3" s="8" t="b">
-        <v>1</v>
+      <c r="L3" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M3" s="3">
         <v>2</v>
@@ -1714,20 +1734,20 @@
         <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="6" t="str">
         <f>IF((C4=""),"",VLOOKUP(C4,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Intake</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I4" s="7" t="b">
         <v>0</v>
@@ -1738,8 +1758,8 @@
       <c r="K4" s="3">
         <v>0</v>
       </c>
-      <c r="L4" s="8" t="b">
-        <v>1</v>
+      <c r="L4" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M4" s="3">
         <v>3</v>
@@ -1753,20 +1773,20 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" s="6" t="str">
         <f>IF((C5=""),"",VLOOKUP(C5,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Intake</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I5" s="7" t="b">
         <v>0</v>
@@ -1777,8 +1797,8 @@
       <c r="K5" s="3">
         <v>0</v>
       </c>
-      <c r="L5" s="8" t="b">
-        <v>0</v>
+      <c r="L5" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M5" s="3">
         <v>4</v>
@@ -1792,20 +1812,20 @@
         <v>1</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" s="6" t="str">
         <f>IF((C6=""),"",VLOOKUP(C6,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Intake</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>36</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I6" s="7" t="b">
         <v>0</v>
@@ -1816,8 +1836,8 @@
       <c r="K6" s="3">
         <v>0</v>
       </c>
-      <c r="L6" s="8" t="b">
-        <v>0</v>
+      <c r="L6" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M6" s="3">
         <v>5</v>
@@ -1844,7 +1864,7 @@
         <v>34</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I7" s="7" t="b">
         <v>0</v>
@@ -1855,8 +1875,8 @@
       <c r="K7" s="3">
         <v>0</v>
       </c>
-      <c r="L7" s="8" t="b">
-        <v>0</v>
+      <c r="L7" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M7" s="3">
         <v>6</v>
@@ -1870,20 +1890,20 @@
         <v>1</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" s="6" t="str">
         <f>IF((C8=""),"",VLOOKUP(C8,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Intake</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I8" s="7" t="b">
         <v>0</v>
@@ -1894,8 +1914,8 @@
       <c r="K8" s="3">
         <v>0</v>
       </c>
-      <c r="L8" s="8" t="b">
-        <v>1</v>
+      <c r="L8" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M8" s="3">
         <v>7</v>
@@ -1909,20 +1929,20 @@
         <v>2</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E9" s="6" t="str">
         <f>IF((C9=""),"",VLOOKUP(C9,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I9" s="7" t="b">
         <v>0</v>
@@ -1933,8 +1953,8 @@
       <c r="K9" s="3">
         <v>0</v>
       </c>
-      <c r="L9" s="8" t="b">
-        <v>1</v>
+      <c r="L9" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M9" s="3">
         <v>8</v>
@@ -1948,20 +1968,20 @@
         <v>2</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E10" s="6" t="str">
         <f>IF((C10=""),"",VLOOKUP(C10,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>36</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I10" s="7" t="b">
         <v>0</v>
@@ -1972,8 +1992,8 @@
       <c r="K10" s="3">
         <v>0</v>
       </c>
-      <c r="L10" s="8" t="b">
-        <v>1</v>
+      <c r="L10" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M10" s="3">
         <v>9</v>
@@ -1987,20 +2007,20 @@
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E11" s="6" t="str">
         <f>IF((C11=""),"",VLOOKUP(C11,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I11" s="7" t="b">
         <v>0</v>
@@ -2011,8 +2031,8 @@
       <c r="K11" s="3">
         <v>0</v>
       </c>
-      <c r="L11" s="8" t="b">
-        <v>0</v>
+      <c r="L11" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M11" s="3">
         <v>10</v>
@@ -2026,20 +2046,20 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E12" s="6" t="str">
         <f>IF((C12=""),"",VLOOKUP(C12,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I12" s="7" t="b">
         <v>0</v>
@@ -2050,8 +2070,8 @@
       <c r="K12" s="3">
         <v>0</v>
       </c>
-      <c r="L12" s="8" t="b">
-        <v>0</v>
+      <c r="L12" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M12" s="3">
         <v>11</v>
@@ -2065,20 +2085,20 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E13" s="6" t="str">
         <f>IF((C13=""),"",VLOOKUP(C13,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>38</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I13" s="7" t="b">
         <v>1</v>
@@ -2089,8 +2109,8 @@
       <c r="K13" s="3">
         <v>30</v>
       </c>
-      <c r="L13" s="8" t="b">
-        <v>0</v>
+      <c r="L13" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M13" s="3">
         <v>12</v>
@@ -2107,20 +2127,20 @@
         <v>2</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E14" s="6" t="str">
         <f>IF((C14=""),"",VLOOKUP(C14,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I14" s="7" t="b">
         <v>0</v>
@@ -2131,8 +2151,8 @@
       <c r="K14" s="3">
         <v>0</v>
       </c>
-      <c r="L14" s="8" t="b">
-        <v>0</v>
+      <c r="L14" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M14" s="3">
         <v>13</v>
@@ -2149,20 +2169,20 @@
         <v>2</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E15" s="6" t="str">
         <f>IF((C15=""),"",VLOOKUP(C15,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I15" s="7" t="b">
         <v>0</v>
@@ -2173,8 +2193,8 @@
       <c r="K15" s="3">
         <v>0</v>
       </c>
-      <c r="L15" s="8" t="b">
-        <v>0</v>
+      <c r="L15" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M15" s="3">
         <v>14</v>
@@ -2191,20 +2211,20 @@
         <v>2</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E16" s="6" t="str">
         <f>IF((C16=""),"",VLOOKUP(C16,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I16" s="7" t="b">
         <v>0</v>
@@ -2215,8 +2235,8 @@
       <c r="K16" s="3">
         <v>0</v>
       </c>
-      <c r="L16" s="8" t="b">
-        <v>0</v>
+      <c r="L16" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M16" s="3">
         <v>15</v>
@@ -2233,20 +2253,20 @@
         <v>2</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E17" s="6" t="str">
         <f>IF((C17=""),"",VLOOKUP(C17,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I17" s="7" t="b">
         <v>0</v>
@@ -2257,8 +2277,8 @@
       <c r="K17" s="3">
         <v>0</v>
       </c>
-      <c r="L17" s="8" t="b">
-        <v>0</v>
+      <c r="L17" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M17" s="3">
         <v>16</v>
@@ -2272,20 +2292,20 @@
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E18" s="6" t="str">
         <f>IF((C18=""),"",VLOOKUP(C18,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>38</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I18" s="7" t="b">
         <v>0</v>
@@ -2296,8 +2316,8 @@
       <c r="K18" s="3">
         <v>0</v>
       </c>
-      <c r="L18" s="8" t="b">
-        <v>0</v>
+      <c r="L18" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M18" s="3">
         <v>17</v>
@@ -2311,20 +2331,20 @@
         <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E19" s="6" t="str">
         <f>IF((C19=""),"",VLOOKUP(C19,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>38</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I19" s="7" t="b">
         <v>0</v>
@@ -2335,8 +2355,8 @@
       <c r="K19" s="3">
         <v>0</v>
       </c>
-      <c r="L19" s="8" t="b">
-        <v>0</v>
+      <c r="L19" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M19" s="3">
         <v>18</v>
@@ -2350,20 +2370,20 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E20" s="6" t="str">
         <f>IF((C20=""),"",VLOOKUP(C20,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>39</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I20" s="7" t="b">
         <v>0</v>
@@ -2374,8 +2394,8 @@
       <c r="K20" s="3">
         <v>0</v>
       </c>
-      <c r="L20" s="8" t="b">
-        <v>0</v>
+      <c r="L20" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M20" s="3">
         <v>19</v>
@@ -2392,20 +2412,20 @@
         <v>2</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E21" s="6" t="str">
         <f>IF((C21=""),"",VLOOKUP(C21,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I21" s="7" t="b">
         <v>0</v>
@@ -2416,8 +2436,8 @@
       <c r="K21" s="3">
         <v>0</v>
       </c>
-      <c r="L21" s="8" t="b">
-        <v>0</v>
+      <c r="L21" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M21" s="3">
         <v>20</v>
@@ -2434,20 +2454,20 @@
         <v>2</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E22" s="6" t="str">
         <f>IF((C22=""),"",VLOOKUP(C22,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I22" s="7" t="b">
         <v>0</v>
@@ -2458,8 +2478,8 @@
       <c r="K22" s="3">
         <v>0</v>
       </c>
-      <c r="L22" s="8" t="b">
-        <v>0</v>
+      <c r="L22" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M22" s="3">
         <v>21</v>
@@ -2473,20 +2493,20 @@
         <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E23" s="6" t="str">
         <f>IF((C23=""),"",VLOOKUP(C23,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>39</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I23" s="7" t="b">
         <v>0</v>
@@ -2497,8 +2517,8 @@
       <c r="K23" s="3">
         <v>0</v>
       </c>
-      <c r="L23" s="8" t="b">
-        <v>0</v>
+      <c r="L23" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M23" s="3">
         <v>22</v>
@@ -2515,20 +2535,20 @@
         <v>2</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E24" s="6" t="str">
         <f>IF((C24=""),"",VLOOKUP(C24,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I24" s="7" t="b">
         <v>0</v>
@@ -2539,8 +2559,8 @@
       <c r="K24" s="3">
         <v>0</v>
       </c>
-      <c r="L24" s="8" t="b">
-        <v>0</v>
+      <c r="L24" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M24" s="3">
         <v>23</v>
@@ -2557,20 +2577,20 @@
         <v>2</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E25" s="6" t="str">
         <f>IF((C25=""),"",VLOOKUP(C25,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I25" s="7" t="b">
         <v>0</v>
@@ -2581,8 +2601,8 @@
       <c r="K25" s="3">
         <v>0</v>
       </c>
-      <c r="L25" s="8" t="b">
-        <v>0</v>
+      <c r="L25" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M25" s="3">
         <v>24</v>
@@ -2590,26 +2610,29 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
+        <v>26</v>
+      </c>
+      <c r="B26" s="3">
         <v>25</v>
       </c>
       <c r="C26" s="8">
         <v>2</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>131</v>
+      <c r="D26" s="18" t="s">
+        <v>130</v>
       </c>
       <c r="E26" s="6" t="str">
         <f>IF((C26=""),"",VLOOKUP(C26,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I26" s="7" t="b">
         <v>0</v>
@@ -2620,16 +2643,16 @@
       <c r="K26" s="3">
         <v>0</v>
       </c>
-      <c r="L26" s="8" t="b">
-        <v>0</v>
+      <c r="L26" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M26" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3">
         <v>25</v>
@@ -2637,8 +2660,8 @@
       <c r="C27" s="8">
         <v>2</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>132</v>
+      <c r="D27" s="19" t="s">
+        <v>131</v>
       </c>
       <c r="E27" s="6" t="str">
         <f>IF((C27=""),"",VLOOKUP(C27,Phases!$A$2:$B$4,2,FALSE))</f>
@@ -2651,7 +2674,7 @@
         <v>35</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I27" s="7" t="b">
         <v>0</v>
@@ -2662,38 +2685,38 @@
       <c r="K27" s="3">
         <v>0</v>
       </c>
-      <c r="L27" s="8" t="b">
-        <v>0</v>
+      <c r="L27" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M27" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" s="3">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C28" s="8">
         <v>2</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>133</v>
+      <c r="D28" s="18" t="s">
+        <v>132</v>
       </c>
       <c r="E28" s="6" t="str">
         <f>IF((C28=""),"",VLOOKUP(C28,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I28" s="7" t="b">
         <v>0</v>
@@ -2704,35 +2727,38 @@
       <c r="K28" s="3">
         <v>0</v>
       </c>
-      <c r="L28" s="8" t="b">
-        <v>0</v>
+      <c r="L28" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M28" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
+        <v>30</v>
+      </c>
+      <c r="B29" s="3">
         <v>28</v>
       </c>
       <c r="C29" s="8">
         <v>2</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>134</v>
+      <c r="D29" s="19" t="s">
+        <v>133</v>
       </c>
       <c r="E29" s="6" t="str">
         <f>IF((C29=""),"",VLOOKUP(C29,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I29" s="7" t="b">
         <v>0</v>
@@ -2743,38 +2769,35 @@
       <c r="K29" s="3">
         <v>0</v>
       </c>
-      <c r="L29" s="8" t="b">
-        <v>0</v>
+      <c r="L29" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M29" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>29</v>
-      </c>
-      <c r="B30" s="3">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C30" s="8">
         <v>2</v>
       </c>
-      <c r="D30" s="18" t="s">
-        <v>135</v>
+      <c r="D30" s="17" t="s">
+        <v>134</v>
       </c>
       <c r="E30" s="6" t="str">
         <f>IF((C30=""),"",VLOOKUP(C30,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I30" s="7" t="b">
         <v>0</v>
@@ -2785,38 +2808,38 @@
       <c r="K30" s="3">
         <v>0</v>
       </c>
-      <c r="L30" s="8" t="b">
-        <v>0</v>
+      <c r="L30" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M30" s="3">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31" s="3">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C31" s="8">
         <v>2</v>
       </c>
-      <c r="D31" s="19" t="s">
-        <v>136</v>
+      <c r="D31" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="E31" s="6" t="str">
         <f>IF((C31=""),"",VLOOKUP(C31,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I31" s="7" t="b">
         <v>0</v>
@@ -2827,35 +2850,38 @@
       <c r="K31" s="3">
         <v>0</v>
       </c>
-      <c r="L31" s="8" t="b">
-        <v>0</v>
+      <c r="L31" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M31" s="3">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
+        <v>33</v>
+      </c>
+      <c r="B32" s="3">
         <v>31</v>
       </c>
       <c r="C32" s="8">
         <v>2</v>
       </c>
-      <c r="D32" s="17" t="s">
-        <v>137</v>
+      <c r="D32" s="19" t="s">
+        <v>136</v>
       </c>
       <c r="E32" s="6" t="str">
         <f>IF((C32=""),"",VLOOKUP(C32,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I32" s="7" t="b">
         <v>0</v>
@@ -2866,38 +2892,35 @@
       <c r="K32" s="3">
         <v>0</v>
       </c>
-      <c r="L32" s="8" t="b">
-        <v>0</v>
+      <c r="L32" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M32" s="3">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>32</v>
-      </c>
-      <c r="B33" s="3">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C33" s="8">
         <v>2</v>
       </c>
-      <c r="D33" s="18" t="s">
-        <v>138</v>
+      <c r="D33" s="17" t="s">
+        <v>114</v>
       </c>
       <c r="E33" s="6" t="str">
         <f>IF((C33=""),"",VLOOKUP(C33,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I33" s="7" t="b">
         <v>0</v>
@@ -2908,38 +2931,38 @@
       <c r="K33" s="3">
         <v>0</v>
       </c>
-      <c r="L33" s="8" t="b">
-        <v>0</v>
+      <c r="L33" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M33" s="3">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" s="3">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C34" s="8">
         <v>2</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>139</v>
+      <c r="D34" s="18" t="s">
+        <v>137</v>
       </c>
       <c r="E34" s="6" t="str">
         <f>IF((C34=""),"",VLOOKUP(C34,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I34" s="7" t="b">
         <v>0</v>
@@ -2950,77 +2973,77 @@
       <c r="K34" s="3">
         <v>0</v>
       </c>
-      <c r="L34" s="8" t="b">
-        <v>0</v>
+      <c r="L34" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M34" s="3">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
+        <v>36</v>
+      </c>
+      <c r="B35" s="3">
         <v>34</v>
       </c>
       <c r="C35" s="8">
         <v>2</v>
       </c>
-      <c r="D35" s="17" t="s">
-        <v>115</v>
+      <c r="D35" s="19" t="s">
+        <v>138</v>
       </c>
       <c r="E35" s="6" t="str">
         <f>IF((C35=""),"",VLOOKUP(C35,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="G35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I35" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="3">
+        <v>0</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M35" s="3">
         <v>36</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="I35" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J35" s="2">
-        <v>0</v>
-      </c>
-      <c r="K35" s="3">
-        <v>0</v>
-      </c>
-      <c r="L35" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="M35" s="3">
-        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>35</v>
-      </c>
-      <c r="B36" s="3">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C36" s="8">
         <v>2</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>140</v>
+      <c r="D36" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E36" s="6" t="str">
         <f>IF((C36=""),"",VLOOKUP(C36,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I36" s="7" t="b">
         <v>0</v>
@@ -3031,77 +3054,74 @@
       <c r="K36" s="3">
         <v>0</v>
       </c>
-      <c r="L36" s="8" t="b">
-        <v>0</v>
+      <c r="L36" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M36" s="3">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C37" s="8">
         <v>2</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>141</v>
+      <c r="D37" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="E37" s="6" t="str">
         <f>IF((C37=""),"",VLOOKUP(C37,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Review</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I37" s="7" t="b">
         <v>0</v>
       </c>
       <c r="J37" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K37" s="3">
         <v>0</v>
       </c>
-      <c r="L37" s="8" t="b">
-        <v>0</v>
+      <c r="L37" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M37" s="3">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C38" s="8">
-        <v>2</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="E38" s="6" t="str">
         <f>IF((C38=""),"",VLOOKUP(C38,Phases!$A$2:$B$4,2,FALSE))</f>
-        <v>Minister's Designation Review</v>
+        <v>Minister's Designation Decision</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I38" s="7" t="b">
         <v>0</v>
@@ -3112,74 +3132,77 @@
       <c r="K38" s="3">
         <v>0</v>
       </c>
-      <c r="L38" s="8" t="b">
-        <v>0</v>
+      <c r="L38" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M38" s="3">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C39" s="8">
-        <v>2</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>118</v>
+        <v>3</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="E39" s="6" t="str">
         <f>IF((C39=""),"",VLOOKUP(C39,Phases!$A$2:$B$4,2,FALSE))</f>
-        <v>Minister's Designation Review</v>
+        <v>Minister's Designation Decision</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I39" s="7" t="b">
         <v>0</v>
       </c>
       <c r="J39" s="2">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="K39" s="3">
         <v>0</v>
       </c>
-      <c r="L39" s="8" t="b">
-        <v>1</v>
+      <c r="L39" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M39" s="3">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="B40" s="3">
+        <v>40</v>
       </c>
       <c r="C40" s="8">
         <v>3</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>142</v>
+      <c r="D40" s="19" t="s">
+        <v>141</v>
       </c>
       <c r="E40" s="6" t="str">
         <f>IF((C40=""),"",VLOOKUP(C40,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I40" s="7" t="b">
         <v>0</v>
@@ -3190,77 +3213,74 @@
       <c r="K40" s="3">
         <v>0</v>
       </c>
-      <c r="L40" s="8" t="b">
-        <v>1</v>
+      <c r="L40" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M40" s="3">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C41" s="8">
         <v>3</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="E41" s="6" t="str">
         <f>IF((C41=""),"",VLOOKUP(C41,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I41" s="7" t="b">
         <v>0</v>
       </c>
       <c r="J41" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K41" s="3">
         <v>0</v>
       </c>
-      <c r="L41" s="8" t="b">
-        <v>1</v>
+      <c r="L41" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M41" s="3">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
-        <v>41</v>
-      </c>
-      <c r="B42" s="3">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C42" s="8">
         <v>3</v>
       </c>
-      <c r="D42" s="19" t="s">
-        <v>144</v>
+      <c r="D42" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="E42" s="6" t="str">
         <f>IF((C42=""),"",VLOOKUP(C42,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I42" s="7" t="b">
         <v>0</v>
@@ -3271,35 +3291,38 @@
       <c r="K42" s="3">
         <v>0</v>
       </c>
-      <c r="L42" s="8" t="b">
-        <v>1</v>
+      <c r="L42" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M42" s="3">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B43" s="3">
+        <v>43</v>
       </c>
       <c r="C43" s="8">
         <v>3</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>114</v>
+      <c r="D43" s="18" t="s">
+        <v>128</v>
       </c>
       <c r="E43" s="6" t="str">
         <f>IF((C43=""),"",VLOOKUP(C43,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I43" s="7" t="b">
         <v>0</v>
@@ -3310,35 +3333,38 @@
       <c r="K43" s="3">
         <v>0</v>
       </c>
-      <c r="L43" s="8" t="b">
-        <v>0</v>
+      <c r="L43" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M43" s="3">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
+        <v>45</v>
+      </c>
+      <c r="B44" s="3">
         <v>43</v>
       </c>
       <c r="C44" s="8">
         <v>3</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>128</v>
+      <c r="D44" s="19" t="s">
+        <v>129</v>
       </c>
       <c r="E44" s="6" t="str">
         <f>IF((C44=""),"",VLOOKUP(C44,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I44" s="7" t="b">
         <v>0</v>
@@ -3349,38 +3375,35 @@
       <c r="K44" s="3">
         <v>0</v>
       </c>
-      <c r="L44" s="8" t="b">
-        <v>0</v>
+      <c r="L44" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M44" s="3">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
-        <v>44</v>
-      </c>
-      <c r="B45" s="3">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C45" s="8">
         <v>3</v>
       </c>
-      <c r="D45" s="18" t="s">
-        <v>129</v>
+      <c r="D45" s="17" t="s">
+        <v>134</v>
       </c>
       <c r="E45" s="6" t="str">
         <f>IF((C45=""),"",VLOOKUP(C45,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I45" s="7" t="b">
         <v>0</v>
@@ -3391,38 +3414,38 @@
       <c r="K45" s="3">
         <v>0</v>
       </c>
-      <c r="L45" s="8" t="b">
-        <v>0</v>
+      <c r="L45" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M45" s="3">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B46" s="3">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C46" s="8">
         <v>3</v>
       </c>
-      <c r="D46" s="19" t="s">
-        <v>130</v>
+      <c r="D46" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="E46" s="6" t="str">
         <f>IF((C46=""),"",VLOOKUP(C46,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I46" s="7" t="b">
         <v>0</v>
@@ -3433,35 +3456,38 @@
       <c r="K46" s="3">
         <v>0</v>
       </c>
-      <c r="L46" s="8" t="b">
-        <v>0</v>
+      <c r="L46" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M46" s="3">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
+        <v>48</v>
+      </c>
+      <c r="B47" s="3">
         <v>46</v>
       </c>
       <c r="C47" s="8">
         <v>3</v>
       </c>
-      <c r="D47" s="17" t="s">
-        <v>137</v>
+      <c r="D47" s="19" t="s">
+        <v>136</v>
       </c>
       <c r="E47" s="6" t="str">
         <f>IF((C47=""),"",VLOOKUP(C47,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I47" s="7" t="b">
         <v>0</v>
@@ -3472,38 +3498,35 @@
       <c r="K47" s="3">
         <v>0</v>
       </c>
-      <c r="L47" s="8" t="b">
-        <v>0</v>
+      <c r="L47" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M47" s="3">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
-        <v>47</v>
-      </c>
-      <c r="B48" s="3">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C48" s="8">
         <v>3</v>
       </c>
-      <c r="D48" s="18" t="s">
-        <v>138</v>
+      <c r="D48" s="17" t="s">
+        <v>114</v>
       </c>
       <c r="E48" s="6" t="str">
         <f>IF((C48=""),"",VLOOKUP(C48,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I48" s="7" t="b">
         <v>0</v>
@@ -3514,38 +3537,38 @@
       <c r="K48" s="3">
         <v>0</v>
       </c>
-      <c r="L48" s="8" t="b">
-        <v>0</v>
+      <c r="L48" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M48" s="3">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49" s="3">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C49" s="8">
         <v>3</v>
       </c>
-      <c r="D49" s="19" t="s">
-        <v>139</v>
+      <c r="D49" s="18" t="s">
+        <v>137</v>
       </c>
       <c r="E49" s="6" t="str">
         <f>IF((C49=""),"",VLOOKUP(C49,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I49" s="7" t="b">
         <v>0</v>
@@ -3556,35 +3579,38 @@
       <c r="K49" s="3">
         <v>0</v>
       </c>
-      <c r="L49" s="8" t="b">
-        <v>0</v>
+      <c r="L49" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M49" s="3">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
+        <v>51</v>
+      </c>
+      <c r="B50" s="3">
         <v>49</v>
       </c>
       <c r="C50" s="8">
         <v>3</v>
       </c>
-      <c r="D50" s="17" t="s">
-        <v>115</v>
+      <c r="D50" s="19" t="s">
+        <v>138</v>
       </c>
       <c r="E50" s="6" t="str">
         <f>IF((C50=""),"",VLOOKUP(C50,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I50" s="7" t="b">
         <v>0</v>
@@ -3595,38 +3621,35 @@
       <c r="K50" s="3">
         <v>0</v>
       </c>
-      <c r="L50" s="8" t="b">
-        <v>0</v>
+      <c r="L50" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M50" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
-        <v>50</v>
-      </c>
-      <c r="B51" s="3">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C51" s="8">
         <v>3</v>
       </c>
-      <c r="D51" s="18" t="s">
-        <v>140</v>
+      <c r="D51" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E51" s="6" t="str">
         <f>IF((C51=""),"",VLOOKUP(C51,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I51" s="7" t="b">
         <v>0</v>
@@ -3637,77 +3660,77 @@
       <c r="K51" s="3">
         <v>0</v>
       </c>
-      <c r="L51" s="8" t="b">
-        <v>0</v>
+      <c r="L51" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="M51" s="3">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
-        <v>51</v>
-      </c>
-      <c r="B52" s="3">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C52" s="8">
         <v>3</v>
       </c>
-      <c r="D52" s="19" t="s">
-        <v>141</v>
+      <c r="D52" s="21" t="s">
+        <v>108</v>
       </c>
       <c r="E52" s="6" t="str">
         <f>IF((C52=""),"",VLOOKUP(C52,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I52" s="7" t="b">
         <v>0</v>
       </c>
       <c r="J52" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K52" s="3">
         <v>0</v>
       </c>
-      <c r="L52" s="8" t="b">
-        <v>0</v>
+      <c r="L52" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M52" s="3">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="B53" s="3">
+        <v>53</v>
       </c>
       <c r="C53" s="8">
         <v>3</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>19</v>
+      <c r="D53" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="E53" s="6" t="str">
         <f>IF((C53=""),"",VLOOKUP(C53,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I53" s="7" t="b">
         <v>0</v>
@@ -3718,138 +3741,57 @@
       <c r="K53" s="3">
         <v>0</v>
       </c>
-      <c r="L53" s="8" t="b">
-        <v>0</v>
+      <c r="L53" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M53" s="3">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
+        <v>55</v>
+      </c>
+      <c r="B54" s="3">
         <v>53</v>
       </c>
       <c r="C54" s="8">
         <v>3</v>
       </c>
-      <c r="D54" s="21" t="s">
-        <v>109</v>
+      <c r="D54" s="19" t="s">
+        <v>143</v>
       </c>
       <c r="E54" s="6" t="str">
         <f>IF((C54=""),"",VLOOKUP(C54,Phases!$A$2:$B$4,2,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I54" s="7" t="b">
         <v>0</v>
       </c>
       <c r="J54" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K54" s="3">
         <v>0</v>
       </c>
-      <c r="L54" s="8" t="b">
-        <v>1</v>
+      <c r="L54" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="M54" s="3">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A55" s="3">
-        <v>54</v>
-      </c>
-      <c r="B55" s="3">
-        <v>53</v>
-      </c>
-      <c r="C55" s="8">
-        <v>3</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="E55" s="6" t="str">
-        <f>IF((C55=""),"",VLOOKUP(C55,Phases!$A$2:$B$4,2,FALSE))</f>
-        <v>Minister's Designation Decision</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="I55" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J55" s="2">
-        <v>0</v>
-      </c>
-      <c r="K55" s="3">
-        <v>0</v>
-      </c>
-      <c r="L55" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M55" s="3">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A56" s="3">
         <v>55</v>
       </c>
-      <c r="B56" s="3">
-        <v>53</v>
-      </c>
-      <c r="C56" s="8">
-        <v>3</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E56" s="6" t="str">
-        <f>IF((C56=""),"",VLOOKUP(C56,Phases!$A$2:$B$4,2,FALSE))</f>
-        <v>Minister's Designation Decision</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H56" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="I56" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J56" s="2">
-        <v>0</v>
-      </c>
-      <c r="K56" s="3">
-        <v>0</v>
-      </c>
-      <c r="L56" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M56" s="3">
-        <v>55</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H56">
+  <conditionalFormatting sqref="H1:H54">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="END">
       <formula>NOT(ISERROR(SEARCH("END",H1)))</formula>
     </cfRule>
@@ -3860,42 +3802,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C94FEBB1-315A-4609-9BCC-2B9E16A284E8}">
-          <x14:formula1>
-            <xm:f>Lookups!$M$3:$M$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>L2:L56</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{52DB5617-9AC6-42B3-A0A1-82418CF13405}">
           <x14:formula1>
             <xm:f>Lookups!$K$3:$K$9</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G56</xm:sqref>
+          <xm:sqref>G2:G54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{65DF4310-1509-4DE8-8535-DCDB722824BD}">
           <x14:formula1>
             <xm:f>Lookups!$Q$3:$Q$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H56</xm:sqref>
+          <xm:sqref>H2:H54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6E633788-78DC-4B8E-B8EE-32416443C2DA}">
           <x14:formula1>
             <xm:f>Lookups!$S$3:$S$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I56</xm:sqref>
+          <xm:sqref>I2:I54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{486DEDE7-BAAD-4F07-BF86-68CC65BA16B7}">
           <x14:formula1>
             <xm:f>Lookups!$I$3:$I$39</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F56</xm:sqref>
+          <xm:sqref>F2:F54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{22B15D01-845E-49E3-A9EB-3C108A48B871}">
           <x14:formula1>
             <xm:f>Phases!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C56</xm:sqref>
+          <xm:sqref>C2:C54</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3948,11 +3884,11 @@
         <v>3</v>
       </c>
       <c r="C2" s="6" t="str">
-        <f>IF((B2=""),"",VLOOKUP(B2,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B2=""),"",VLOOKUP(B2,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -3966,11 +3902,11 @@
         <v>3</v>
       </c>
       <c r="C3" s="6" t="str">
-        <f>IF((B3=""),"",VLOOKUP(B3,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B3=""),"",VLOOKUP(B3,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -3984,11 +3920,11 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="str">
-        <f>IF((B4=""),"",VLOOKUP(B4,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B4=""),"",VLOOKUP(B4,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E4" s="3">
         <v>3</v>
@@ -4002,11 +3938,11 @@
         <v>3</v>
       </c>
       <c r="C5" s="6" t="str">
-        <f>IF((B5=""),"",VLOOKUP(B5,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B5=""),"",VLOOKUP(B5,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Initial Review</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
@@ -4020,11 +3956,11 @@
         <v>5</v>
       </c>
       <c r="C6" s="6" t="str">
-        <f>IF((B6=""),"",VLOOKUP(B6,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B6=""),"",VLOOKUP(B6,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E6" s="3">
         <v>5</v>
@@ -4038,11 +3974,11 @@
         <v>8</v>
       </c>
       <c r="C7" s="6" t="str">
-        <f>IF((B7=""),"",VLOOKUP(B7,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B7=""),"",VLOOKUP(B7,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Received</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E7" s="3">
         <v>6</v>
@@ -4056,11 +3992,11 @@
         <v>9</v>
       </c>
       <c r="C8" s="6" t="str">
-        <f>IF((B8=""),"",VLOOKUP(B8,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B8=""),"",VLOOKUP(B8,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Delegation of Decision</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E8" s="3">
         <v>7</v>
@@ -4074,11 +4010,11 @@
         <v>9</v>
       </c>
       <c r="C9" s="6" t="str">
-        <f>IF((B9=""),"",VLOOKUP(B9,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B9=""),"",VLOOKUP(B9,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Delegation of Decision</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E9" s="3">
         <v>8</v>
@@ -4092,11 +4028,11 @@
         <v>31</v>
       </c>
       <c r="C10" s="6" t="str">
-        <f>IF((B10=""),"",VLOOKUP(B10,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B10=""),"",VLOOKUP(B10,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Process Terminated s.39(d)</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E10" s="3">
         <v>9</v>
@@ -4110,11 +4046,11 @@
         <v>34</v>
       </c>
       <c r="C11" s="6" t="str">
-        <f>IF((B11=""),"",VLOOKUP(B11,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B11=""),"",VLOOKUP(B11,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E11" s="3">
         <v>10</v>
@@ -4128,11 +4064,11 @@
         <v>46</v>
       </c>
       <c r="C12" s="6" t="str">
-        <f>IF((B12=""),"",VLOOKUP(B12,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B12=""),"",VLOOKUP(B12,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Process Terminated s.39(d)</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E12" s="3">
         <v>11</v>
@@ -4146,11 +4082,11 @@
         <v>49</v>
       </c>
       <c r="C13" s="6" t="str">
-        <f>IF((B13=""),"",VLOOKUP(B13,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B13=""),"",VLOOKUP(B13,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Application Withdrawn</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E13" s="3">
         <v>12</v>
@@ -4164,11 +4100,11 @@
         <v>53</v>
       </c>
       <c r="C14" s="6" t="str">
-        <f>IF((B14=""),"",VLOOKUP(B14,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B14=""),"",VLOOKUP(B14,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E14" s="3">
         <v>13</v>
@@ -4182,11 +4118,11 @@
         <v>53</v>
       </c>
       <c r="C15" s="6" t="str">
-        <f>IF((B15=""),"",VLOOKUP(B15,Events!$A$2:$D$56,4,FALSE))</f>
+        <f>IF((B15=""),"",VLOOKUP(B15,Events!$A$2:$D$54,4,FALSE))</f>
         <v>Minister's Designation Decision</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E15" s="3">
         <v>14</v>
@@ -4199,7 +4135,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{104E34E7-1558-4F0E-B347-AA979B498781}">
           <x14:formula1>
-            <xm:f>Events!$A$2:$A$56</xm:f>
+            <xm:f>Events!$A$2:$A$54</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B15</xm:sqref>
         </x14:dataValidation>
@@ -4214,10 +4150,10 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4267,13 +4203,13 @@
         <v>Draft Minister's Designation Application is "incomplete"</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -4291,13 +4227,13 @@
         <v>Draft Minister's Designation Application is "incomplete"</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -4315,13 +4251,13 @@
         <v>Draft Minister's Designation Application is for an "eligible" project</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
@@ -4339,13 +4275,13 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -4363,13 +4299,13 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
@@ -4387,13 +4323,13 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
@@ -4411,13 +4347,13 @@
         <v>Project submitted exceeds RPR threshold(s)</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="G8" s="3">
         <v>7</v>
@@ -4435,13 +4371,13 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
@@ -4459,13 +4395,13 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
@@ -4483,13 +4419,13 @@
         <v>Project submitted exceeds RPR threshold(s) and is Substantially Started</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
@@ -4507,13 +4443,13 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
@@ -4531,13 +4467,13 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
@@ -4555,13 +4491,13 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>66</v>
+        <v>180</v>
       </c>
       <c r="G14" s="3">
         <v>13</v>
@@ -4579,13 +4515,13 @@
         <v>Applicant withdraws Submission from the Minister's Designation process</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G15" s="3">
         <v>14</v>
@@ -4603,13 +4539,13 @@
         <v>Starts the "clock" for Minister's Designation</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G16" s="3">
         <v>15</v>
@@ -4627,13 +4563,13 @@
         <v>Minister is delegated to make the final Minister's Designation Decision</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G17" s="3">
         <v>16</v>
@@ -4651,13 +4587,13 @@
         <v>CEAO is delegated to make the final Minister's Designation Decision</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G18" s="3">
         <v>17</v>
@@ -4675,13 +4611,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="G19" s="3">
         <v>18</v>
@@ -4699,13 +4635,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G20" s="3">
         <v>19</v>
@@ -4723,13 +4659,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G21" s="3">
         <v>20</v>
@@ -4747,13 +4683,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G22" s="3">
         <v>21</v>
@@ -4771,13 +4707,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="G23" s="3">
         <v>22</v>
@@ -4795,13 +4731,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G24" s="3">
         <v>23</v>
@@ -4819,13 +4755,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G25" s="3">
         <v>24</v>
@@ -4843,13 +4779,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G26" s="3">
         <v>25</v>
@@ -4867,13 +4803,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="G27" s="3">
         <v>26</v>
@@ -4891,13 +4827,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G28" s="3">
         <v>27</v>
@@ -4915,13 +4851,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G29" s="3">
         <v>28</v>
@@ -4939,13 +4875,13 @@
         <v>Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G30" s="3">
         <v>29</v>
@@ -4963,13 +4899,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="G31" s="3">
         <v>30</v>
@@ -4987,13 +4923,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G32" s="3">
         <v>31</v>
@@ -5011,13 +4947,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G33" s="3">
         <v>32</v>
@@ -5035,13 +4971,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G34" s="3">
         <v>33</v>
@@ -5059,13 +4995,13 @@
         <v>Decision Maker Designates Project as Reviewable</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G35" s="3">
         <v>34</v>
@@ -5083,13 +5019,13 @@
         <v>Decision Maker Designates Project as Reviewable</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="G36" s="3">
         <v>35</v>
@@ -5107,13 +5043,13 @@
         <v>Decision Maker Declines to Designate Project as Reviewable</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G37" s="3">
         <v>36</v>
@@ -5131,13 +5067,13 @@
         <v>Decision Maker Declines to Designate Project as Reviewable</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G38" s="3">
         <v>37</v>
@@ -5230,11 +5166,11 @@
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R2" s="5"/>
       <c r="S2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -5291,7 +5227,7 @@
         <v>34</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>34</v>
@@ -5303,7 +5239,7 @@
         <v>52</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S3" s="2" t="b">
         <v>1</v>
@@ -5323,7 +5259,7 @@
         <v>34</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>35</v>
@@ -5335,7 +5271,7 @@
         <v>53</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S4" s="2" t="b">
         <v>0</v>
@@ -5352,7 +5288,7 @@
         <v>34</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>36</v>
@@ -5361,7 +5297,7 @@
         <v>50</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.3">
@@ -5372,7 +5308,7 @@
         <v>34</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>37</v>
@@ -5383,13 +5319,13 @@
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>38</v>
@@ -5406,7 +5342,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>39</v>
@@ -5417,13 +5353,13 @@
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>40</v>
@@ -5440,7 +5376,7 @@
         <v>34</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>51</v>
@@ -5466,7 +5402,7 @@
         <v>34</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O12" s="9"/>
     </row>
@@ -5478,7 +5414,7 @@
         <v>39</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O13" s="9"/>
     </row>
@@ -5490,7 +5426,7 @@
         <v>39</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O14" s="9"/>
     </row>
@@ -5502,7 +5438,7 @@
         <v>40</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O15" s="9"/>
     </row>
@@ -5514,7 +5450,7 @@
         <v>40</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="8:9" x14ac:dyDescent="0.3">
@@ -5522,7 +5458,7 @@
         <v>36</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="8:9" x14ac:dyDescent="0.3">
@@ -5530,7 +5466,7 @@
         <v>36</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="8:9" x14ac:dyDescent="0.3">
@@ -5538,7 +5474,7 @@
         <v>36</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="8:9" x14ac:dyDescent="0.3">
@@ -5546,7 +5482,7 @@
         <v>36</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="8:9" x14ac:dyDescent="0.3">
@@ -5554,7 +5490,7 @@
         <v>36</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="8:9" x14ac:dyDescent="0.3">
@@ -5562,7 +5498,7 @@
         <v>36</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="8:9" x14ac:dyDescent="0.3">
@@ -5570,7 +5506,7 @@
         <v>36</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="8:9" x14ac:dyDescent="0.3">
@@ -5578,7 +5514,7 @@
         <v>36</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="8:9" x14ac:dyDescent="0.3">
@@ -5594,7 +5530,7 @@
         <v>38</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="8:9" x14ac:dyDescent="0.3">
@@ -5602,7 +5538,7 @@
         <v>38</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="8:9" x14ac:dyDescent="0.3">
@@ -5610,7 +5546,7 @@
         <v>38</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="8:9" x14ac:dyDescent="0.3">
@@ -5626,7 +5562,7 @@
         <v>35</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="8:9" x14ac:dyDescent="0.3">
@@ -5634,7 +5570,7 @@
         <v>35</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.3">
@@ -5642,7 +5578,7 @@
         <v>35</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="8:9" x14ac:dyDescent="0.3">
@@ -5650,7 +5586,7 @@
         <v>35</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="8:9" x14ac:dyDescent="0.3">
@@ -5666,7 +5602,7 @@
         <v>37</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="8:9" x14ac:dyDescent="0.3">
@@ -5674,7 +5610,7 @@
         <v>37</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="8:9" x14ac:dyDescent="0.3">
@@ -5682,7 +5618,7 @@
         <v>37</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="8:9" x14ac:dyDescent="0.3">
@@ -5690,7 +5626,7 @@
         <v>37</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="8:9" x14ac:dyDescent="0.3">

</xml_diff>